<commit_message>
Coluna com fórmula para apresentar quantidade real disponível adicionada
</commit_message>
<xml_diff>
--- a/CONTROLE ALMOXARIFADO/CONTROLE DE INSUMOS.xlsx
+++ b/CONTROLE ALMOXARIFADO/CONTROLE DE INSUMOS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Material</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>CONTROLE DE INSUMOS</t>
+  </si>
+  <si>
+    <t>Quantidade restante</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -270,22 +273,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,6 +364,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -617,51 +681,57 @@
     <col min="2" max="2" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="21.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7" ht="15">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
@@ -673,15 +743,19 @@
       <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
+        <f>B4-D4</f>
+        <v>135</v>
+      </c>
+      <c r="F4" s="3">
         <v>155</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" ht="15">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
@@ -693,15 +767,19 @@
       <c r="D5" s="2">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E13" si="0">B5-D5</f>
+        <v>190</v>
+      </c>
+      <c r="F5" s="3">
         <v>156</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7" ht="15">
+      <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
@@ -713,15 +791,19 @@
       <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="F6" s="3">
         <v>157</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" ht="15">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
@@ -733,15 +815,19 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="F7" s="3">
         <v>158</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" ht="15">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
@@ -753,15 +839,19 @@
       <c r="D8" s="2">
         <v>10</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="F8" s="3">
         <v>159</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:7" ht="15">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
@@ -773,15 +863,19 @@
       <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F9" s="3">
         <v>160</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7" ht="15">
+      <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
@@ -793,15 +887,19 @@
       <c r="D10" s="2">
         <v>2</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F10" s="3">
         <v>161</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:7" ht="15">
+      <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
@@ -813,15 +911,19 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F11" s="3">
         <v>162</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" ht="15">
+      <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
@@ -833,36 +935,44 @@
       <c r="D12" s="2">
         <v>10</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F12" s="3">
         <v>163</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="9">
         <v>20</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F13" s="5">
         <v>164</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A1:G2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>